<commit_message>
Updated Product Backlog to sort by priority.
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
   <si>
     <t>PRODUCT BACKLOG</t>
   </si>
@@ -58,19 +58,40 @@
     <t>S</t>
   </si>
   <si>
+    <t>As a user, I need to be able to see what action a person has taken (such as create, delete)</t>
+  </si>
+  <si>
+    <t>Data classification</t>
+  </si>
+  <si>
     <t>As a developer, I need to be able to use the API to get the ID of a change</t>
+  </si>
+  <si>
+    <t>As a user, I need to be able to see the individual changes data for a file represented in the form of a histogram</t>
+  </si>
+  <si>
+    <t>Graphical Representation</t>
+  </si>
+  <si>
+    <t>As a user, I need to be able to see the revision data being represented in the form of a pie chart</t>
+  </si>
+  <si>
+    <t>As a user, I need to be able to see the revision data for files within a team drive, even when a folder exists in said drive</t>
+  </si>
+  <si>
+    <t>As a developer, I need to be able to retrieve the files inside a folder</t>
   </si>
   <si>
     <t>As a developer, I need to be able to use the API to get the time of change</t>
   </si>
   <si>
-    <t>As a developer, I need to be able to use the API to get the name of the user who made the change</t>
+    <t>As a developer, I need to be able to retrieve the number of actions that a user has made to a file</t>
   </si>
   <si>
-    <t>As a developer, I need to be able to retrieve the changes that a user has made to a file</t>
+    <t>Data retrieval</t>
   </si>
   <si>
-    <t>XL</t>
+    <t>As a developer, I need to be able to use the API to get the name of the user who made the change</t>
   </si>
   <si>
     <t>As a user, I need to see changes to a file in chronological order in the form of a timeline provided I have permission to access that file</t>
@@ -100,10 +121,19 @@
     <t>Action used to make changes</t>
   </si>
   <si>
+    <t>XL</t>
+  </si>
+  <si>
     <t>As a user, I want the interface to look neat and clean so that I can look at and understand the contents with ease</t>
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a user, I need to be able to see the revision information on a webpage </t>
+  </si>
+  <si>
+    <t>Printing data on the webpage</t>
   </si>
 </sst>
 </file>
@@ -209,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -245,14 +275,32 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
@@ -380,14 +428,14 @@
       <c r="A8" s="8">
         <v>4.0</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>10</v>
+      <c r="C8" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>11</v>
@@ -398,10 +446,10 @@
         <v>5.0</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>10</v>
@@ -414,14 +462,14 @@
       <c r="A10" s="8">
         <v>6.0</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="10">
-        <v>4.0</v>
+      <c r="B10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2.0</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>11</v>
@@ -431,31 +479,31 @@
       <c r="A11" s="8">
         <v>7.0</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="D11" s="12" t="s">
-        <v>10</v>
+      <c r="B11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="8">
         <v>8.0</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="B12" s="13" t="s">
         <v>21</v>
+      </c>
+      <c r="C12" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>11</v>
@@ -465,16 +513,16 @@
       <c r="A13" s="8">
         <v>9.0</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="11" t="s">
+      <c r="C13" s="14">
+        <v>2.0</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>11</v>
       </c>
     </row>
@@ -483,13 +531,13 @@
         <v>10.0</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>21</v>
+        <v>3.0</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>11</v>
@@ -500,13 +548,13 @@
         <v>11.0</v>
       </c>
       <c r="B15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="D15" s="10" t="s">
         <v>25</v>
-      </c>
-      <c r="C15" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>26</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>11</v>
@@ -517,70 +565,136 @@
         <v>12.0</v>
       </c>
       <c r="B16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C17" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10">
         <v>8.0</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D21" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="17">
+        <v>9.0</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="13">
-        <v>13.0</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="15">
-        <v>9.0</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="E22" s="11" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="A23" s="18">
+        <v>19.0</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="20">
+        <v>10.0</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="5"/>

</xml_diff>